<commit_message>
update natural products with Alaska data
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="107">
   <si>
     <t>Layer</t>
   </si>
@@ -312,6 +312,48 @@
   </si>
   <si>
     <t>http://www.fiskeridir.no/Akvakultur/Statistikk-akvakultur/Statistiske-publikasjoner/Statistikk-for-akvakultur</t>
+  </si>
+  <si>
+    <t>np_harvest_individuals_arc2016</t>
+  </si>
+  <si>
+    <t>FAO marine mammal capture data</t>
+  </si>
+  <si>
+    <t>http://www.nmfs.noaa.gov/pr/sars/pdf/alaska2014_summary_final.pdf</t>
+  </si>
+  <si>
+    <t>Estimated total mortality of individuals per year</t>
+  </si>
+  <si>
+    <t>No. individuals captured by country (seals for pelts, walrus and narwhal for ivory)</t>
+  </si>
+  <si>
+    <t>FAO catch statistics. Large seal population around Jan Mayen but catch reporting goes to Norway. Seal stocks are managed jointly by Russia/Norway and quotas from ICES.</t>
+  </si>
+  <si>
+    <t>V small licenced catch in Svalbard.  Can't get statistics so N/A</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>NP_quotas</t>
+  </si>
+  <si>
+    <t>Quotas set for NP products</t>
+  </si>
+  <si>
+    <t>No quotas set - have limited Potential Biological Removal data for a couple of species</t>
+  </si>
+  <si>
+    <t>Quotas set jointly by Russia/Norway as advised by ICES- still trying to get hold</t>
+  </si>
+  <si>
+    <t>No quotas for seal - obtained quotas for Walrus and 2015/2016 for narwhal - trying to get further back in time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAO statistics. </t>
   </si>
 </sst>
 </file>
@@ -696,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,6 +1077,58 @@
       </c>
       <c r="J8" s="2" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1064,6 +1158,7 @@
     <hyperlink ref="L7" r:id="rId23"/>
     <hyperlink ref="N7" r:id="rId24"/>
     <hyperlink ref="J8" r:id="rId25"/>
+    <hyperlink ref="H9" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update natural products with Norway/Russia seal catch and quota, pacific walrus etc
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -24,27 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="123">
   <si>
     <t>Layer</t>
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Russia data</t>
-  </si>
-  <si>
-    <t>Canada data</t>
-  </si>
-  <si>
-    <t>USA data</t>
-  </si>
-  <si>
-    <t>Norway data</t>
-  </si>
-  <si>
-    <t>Greenland data</t>
   </si>
   <si>
     <t>le_population_arc2016</t>
@@ -88,9 +73,6 @@
   </si>
   <si>
     <t>https://www.ssb.no/statistikkbanken/selectvarval/Define.asp?subjectcode=&amp;ProductId=&amp;MainTable=Rd0002AaX5&amp;nvl=&amp;PLanguage=1&amp;nyTmpVar=true&amp;CMSSubjectArea=befolkning&amp;KortNavnWeb=folkemengde&amp;StatVariant=</t>
-  </si>
-  <si>
-    <t>Svlbard Data</t>
   </si>
   <si>
     <t>Population data for Svalbard</t>
@@ -249,9 +231,6 @@
     <t>Average income per capita - same for all sectors</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Needs PPP adjusting and exchange rate adjusting</t>
   </si>
   <si>
@@ -259,9 +238,6 @@
   </si>
   <si>
     <t>Production by sector</t>
-  </si>
-  <si>
-    <t>Needs multiplier adding to account for indirect employment?</t>
   </si>
   <si>
     <t>http://www.gks.ru/wps/wcm/connect/rosstat_main/rosstat/ru/statistics/accounts/#</t>
@@ -317,24 +293,12 @@
     <t>np_harvest_individuals_arc2016</t>
   </si>
   <si>
-    <t>FAO marine mammal capture data</t>
-  </si>
-  <si>
     <t>http://www.nmfs.noaa.gov/pr/sars/pdf/alaska2014_summary_final.pdf</t>
   </si>
   <si>
-    <t>Estimated total mortality of individuals per year</t>
-  </si>
-  <si>
     <t>No. individuals captured by country (seals for pelts, walrus and narwhal for ivory)</t>
   </si>
   <si>
-    <t>FAO catch statistics. Large seal population around Jan Mayen but catch reporting goes to Norway. Seal stocks are managed jointly by Russia/Norway and quotas from ICES.</t>
-  </si>
-  <si>
-    <t>V small licenced catch in Svalbard.  Can't get statistics so N/A</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -344,16 +308,108 @@
     <t>Quotas set for NP products</t>
   </si>
   <si>
-    <t>No quotas set - have limited Potential Biological Removal data for a couple of species</t>
-  </si>
-  <si>
-    <t>Quotas set jointly by Russia/Norway as advised by ICES- still trying to get hold</t>
-  </si>
-  <si>
-    <t>No quotas for seal - obtained quotas for Walrus and 2015/2016 for narwhal - trying to get further back in time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAO statistics. </t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Russia data (Region 4)</t>
+  </si>
+  <si>
+    <t>Canada data (Nunavut 2, NWT 3)</t>
+  </si>
+  <si>
+    <t>USA data (Region 1)</t>
+  </si>
+  <si>
+    <t>Norway data (Region 6)</t>
+  </si>
+  <si>
+    <t>Greenland data (West 8, East 9)</t>
+  </si>
+  <si>
+    <t>Svlbard Data (Region 5)</t>
+  </si>
+  <si>
+    <t>Jan Mayen (Region 7)</t>
+  </si>
+  <si>
+    <t>Jan Mayen Links</t>
+  </si>
+  <si>
+    <t>No quotas for seal - obtained quotas for Walrus and narwhal</t>
+  </si>
+  <si>
+    <t>http://www.businessingreenland.gl/~/media/Fiskeri%20og%20fangst/Hvalros%20Fangsttal%202006-2016_DK-2.pdf?la=da
+http://www.businessingreenland.gl/~/media/Fiskeri%20og%20fangst/smaa%20hvaler%20DK%202006-2015.pdf?la=da</t>
+  </si>
+  <si>
+    <t>FAO data for whole of Canada but not really relevant - as large commercial harvest outside NWT/Nunavut. Got Nunavut Narwhal data. No Narwhal catch in NWT</t>
+  </si>
+  <si>
+    <t>Nunavut Narhwal quota. No seal quota for NWT/Nunavut</t>
+  </si>
+  <si>
+    <t>Narhwal integrated management plan</t>
+  </si>
+  <si>
+    <t>Estimated total mortality of individuals per year for seals. Walrus data obtained from FWS</t>
+  </si>
+  <si>
+    <t>No quotas set for seals or walrus.</t>
+  </si>
+  <si>
+    <t>http://www.ices.dk/sites/pub/Publication%20Reports/Advice/2013/Special%20requests/Norway_Harp%20and%20Hooded%20Seals.pdf</t>
+  </si>
+  <si>
+    <t>West Ice (Jan Mayen) catches and East Ice (Norway) quotas</t>
+  </si>
+  <si>
+    <t>ICES Quotas for Harp and Hooded Seals</t>
+  </si>
+  <si>
+    <t>West Ice (Jan Mayen) catches for harp and hooded seal East Ice (Norway) catches</t>
+  </si>
+  <si>
+    <t>West Ice (Jan Mayen) catches for harp and hooded sea</t>
+  </si>
+  <si>
+    <t>West Ice (Jan Mayen) quota for harp and hooded sea</t>
+  </si>
+  <si>
+    <t>FAO statistics. Walrus and Narwhal catches found</t>
+  </si>
+  <si>
+    <t>NP_Struck and Lost rate</t>
+  </si>
+  <si>
+    <t>Walrus 42% struck and lost - multiply by 1.42</t>
+  </si>
+  <si>
+    <t>https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf</t>
+  </si>
+  <si>
+    <t>Narwhal 28% struck and lost - multiply by 1.42</t>
+  </si>
+  <si>
+    <t>http://www.nwmb.com/en/public-hearings-a-meetings/workshops/march-2013-marine-mammal-struck-and-loss-in-nunavut/5698-workshop-summary-marine-mammal-struck-and-loss-in-nunavut-eng/file</t>
+  </si>
+  <si>
+    <t>http://www.ifaw.org/sites/default/files/2007_An%20illustrated%20guide%20to%20the%20tool%20used%20to%20kill%20seals%20in%20the%20canadas%20commercial%20seal%20hunt.pdf</t>
+  </si>
+  <si>
+    <t>Loss rates for young seals taken on the ice are estimated
+to vary from 0% to 1.9%, and from 0% to 10.0% when
+shot in the water. Seals greater than one year of age have
+loss rates of 0%-4.9% when taken on the ice and
+13.8%-50.0% when shot in the water (Sjare and
+Stenson 2002). The government of Canada currently
+estimates struck and lost rates at 5% for seals under one
+year of age, and 50% for older seals (Stenson 2005).</t>
+  </si>
+  <si>
+    <t>Struck and lost rates only need to be implemented for where quotas aren't present - as these will have already been factored in to the quota</t>
+  </si>
+  <si>
+    <t>Harp and Hooded Seal catches. Contacted person about pacific walrus catch</t>
   </si>
 </sst>
 </file>
@@ -738,10 +794,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,10 +816,11 @@
     <col min="11" max="11" width="15.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="1"/>
     <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="25.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -770,365 +828,445 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="5" t="s">
+    </row>
+    <row r="3" spans="1:16" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>72</v>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
+    <row r="4" spans="1:16" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="194.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>36</v>
+      <c r="F6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>36</v>
+    <row r="7" spans="1:16" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="194.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>73</v>
+    <row r="8" spans="1:16" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="1" t="s">
+    <row r="9" spans="1:16" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>87</v>
+      <c r="I9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:16" ht="151.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>92</v>
+      <c r="M10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>105</v>
+    <row r="11" spans="1:16" ht="177" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1297,13 @@
     <hyperlink ref="N7" r:id="rId24"/>
     <hyperlink ref="J8" r:id="rId25"/>
     <hyperlink ref="H9" r:id="rId26"/>
+    <hyperlink ref="N10" r:id="rId27" display="http://www.businessingreenland.gl/~/media/Fiskeri%20og%20fangst/Hvalros%20Fangsttal%202006-2016_DK-2.pdf?la=da"/>
+    <hyperlink ref="N9" r:id="rId28" display="http://www.businessingreenland.gl/~/media/Fiskeri%20og%20fangst/Hvalros%20Fangsttal%202006-2016_DK-2.pdf?la=da"/>
+    <hyperlink ref="H11" r:id="rId29"/>
+    <hyperlink ref="F11" r:id="rId30"/>
+    <hyperlink ref="J11" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update natural products data
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -348,18 +348,12 @@
     <t>Estimated total mortality of individuals per year for seals. Walrus data obtained from FWS</t>
   </si>
   <si>
-    <t>No quotas set for seals or walrus.</t>
-  </si>
-  <si>
     <t>http://www.ices.dk/sites/pub/Publication%20Reports/Advice/2013/Special%20requests/Norway_Harp%20and%20Hooded%20Seals.pdf</t>
   </si>
   <si>
     <t>West Ice (Jan Mayen) catches and East Ice (Norway) quotas</t>
   </si>
   <si>
-    <t>ICES Quotas for Harp and Hooded Seals</t>
-  </si>
-  <si>
     <t>West Ice (Jan Mayen) catches for harp and hooded seal East Ice (Norway) catches</t>
   </si>
   <si>
@@ -375,13 +369,7 @@
     <t>NP_Struck and Lost rate</t>
   </si>
   <si>
-    <t>Walrus 42% struck and lost - multiply by 1.42</t>
-  </si>
-  <si>
     <t>https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf</t>
-  </si>
-  <si>
-    <t>Narwhal 28% struck and lost - multiply by 1.42</t>
   </si>
   <si>
     <t>http://www.nwmb.com/en/public-hearings-a-meetings/workshops/march-2013-marine-mammal-struck-and-loss-in-nunavut/5698-workshop-summary-marine-mammal-struck-and-loss-in-nunavut-eng/file</t>
@@ -403,9 +391,6 @@
     <t>Struck and lost rates only need to be implemented for where quotas aren't present - as these will have already been factored in to the quota</t>
   </si>
   <si>
-    <t>Harp and Hooded Seal catches. Contacted person about pacific walrus catch</t>
-  </si>
-  <si>
     <t>tr_jobs_total_arc2016</t>
   </si>
   <si>
@@ -449,6 +434,21 @@
   </si>
   <si>
     <t>Same data for whole of Greenland - split equally between West and East</t>
+  </si>
+  <si>
+    <t>No quotas set for seals or walrus. PBR for pacific walrus used as sustainable limit from here https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf</t>
+  </si>
+  <si>
+    <t>Narwhal 28% struck and lost - multiply by 1.28</t>
+  </si>
+  <si>
+    <t>Walrus 42% struck and lost - figures multiplied by 1.42 as reference is PBR not quota</t>
+  </si>
+  <si>
+    <t>ICES Quotas for Harp and Hooded Seals. Pacific Walrus PBR - joint with USA</t>
+  </si>
+  <si>
+    <t>Harp and Hooded Seal catches. Contacted person about pacific walrus catch - have 5 years of data included 2006-2010</t>
   </si>
 </sst>
 </file>
@@ -842,8 +842,8 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,10 +1238,10 @@
         <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>100</v>
@@ -1256,10 +1256,10 @@
         <v>84</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>86</v>
@@ -1268,16 +1268,16 @@
         <v>86</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>99</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="151.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1288,10 +1288,10 @@
         <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>101</v>
@@ -1300,13 +1300,13 @@
         <v>102</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>86</v>
@@ -1321,47 +1321,47 @@
         <v>99</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="G11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1383,13 +1383,13 @@
     </row>
     <row r="13" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1411,13 +1411,13 @@
     </row>
     <row r="14" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1433,31 +1433,31 @@
     </row>
     <row r="15" spans="1:16" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
update meta data doc
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -436,19 +436,20 @@
     <t>Same data for whole of Greenland - split equally between West and East</t>
   </si>
   <si>
-    <t>No quotas set for seals or walrus. PBR for pacific walrus used as sustainable limit from here https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf</t>
-  </si>
-  <si>
     <t>Narwhal 28% struck and lost - multiply by 1.28</t>
   </si>
   <si>
-    <t>Walrus 42% struck and lost - figures multiplied by 1.42 as reference is PBR not quota</t>
-  </si>
-  <si>
     <t>ICES Quotas for Harp and Hooded Seals. Pacific Walrus PBR - joint with USA</t>
   </si>
   <si>
     <t>Harp and Hooded Seal catches. Contacted person about pacific walrus catch - have 5 years of data included 2006-2010</t>
+  </si>
+  <si>
+    <t>Walrus 42% struck and lost - figures multiplied by 1.42 as reference is PBR not quota. Spotted seal struck and lost rate 1.50 - as per Canadian struck and lost. Multiplied in excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No quotas set for seals or walrus. PBR for pacific walrus used as sustainable limit from here https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf
+No PBR for ringed, bearded, ribbon seals </t>
   </si>
 </sst>
 </file>
@@ -843,7 +844,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,7 +1239,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>104</v>
@@ -1288,7 +1289,7 @@
         <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>104</v>
@@ -1300,7 +1301,7 @@
         <v>102</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>105</v>
@@ -1335,13 +1336,13 @@
         <v>115</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>112</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
update NP with russian walrus data
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -442,14 +442,14 @@
     <t>ICES Quotas for Harp and Hooded Seals. Pacific Walrus PBR - joint with USA</t>
   </si>
   <si>
-    <t>Harp and Hooded Seal catches. Contacted person about pacific walrus catch - have 5 years of data included 2006-2010</t>
-  </si>
-  <si>
     <t>Walrus 42% struck and lost - figures multiplied by 1.42 as reference is PBR not quota. Spotted seal struck and lost rate 1.50 - as per Canadian struck and lost. Multiplied in excel</t>
   </si>
   <si>
     <t xml:space="preserve">No quotas set for seals or walrus. PBR for pacific walrus used as sustainable limit from here https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf
 No PBR for ringed, bearded, ribbon seals </t>
+  </si>
+  <si>
+    <t>Harp and Hooded Seal catches. Walrus catch included from ChukotTIRO</t>
   </si>
 </sst>
 </file>
@@ -844,7 +844,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1239,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>104</v>
@@ -1301,7 +1301,7 @@
         <v>102</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>105</v>
@@ -1342,7 +1342,7 @@
         <v>112</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
add arctic_land shape files from Jamie
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -843,8 +843,8 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update NP for making goal model
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -296,9 +296,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>NP_quotas</t>
-  </si>
-  <si>
     <t>Quotas set for NP products</t>
   </si>
   <si>
@@ -439,17 +436,20 @@
     <t>Narwhal 28% struck and lost - multiply by 1.28</t>
   </si>
   <si>
-    <t>ICES Quotas for Harp and Hooded Seals. Pacific Walrus PBR - joint with USA</t>
-  </si>
-  <si>
     <t>Walrus 42% struck and lost - figures multiplied by 1.42 as reference is PBR not quota. Spotted seal struck and lost rate 1.50 - as per Canadian struck and lost. Multiplied in excel</t>
   </si>
   <si>
-    <t xml:space="preserve">No quotas set for seals or walrus. PBR for pacific walrus used as sustainable limit from here https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf
+    <t>Harp and Hooded Seal catches. Walrus catch included from ChukotTIRO</t>
+  </si>
+  <si>
+    <t>NP_harvest_quota_arc2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No quotas set for seals or walrus. PBR for pacific walrus used as sustainable limit from here. Assumed PBR split equally with Russia https://www.fws.gov/alaska/fisheries/mmm/stock/Revised_April_2014_Pacific_Walrus_SAR.pdf
 No PBR for ringed, bearded, ribbon seals </t>
   </si>
   <si>
-    <t>Harp and Hooded Seal catches. Walrus catch included from ChukotTIRO</t>
+    <t>ICES Quotas for Harp and Hooded Seals. Pacific Walrus PBR - joint with USA - assume this is split equally</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,46 +874,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>17</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>44</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="144" customHeight="1" x14ac:dyDescent="0.3">
@@ -960,10 +960,10 @@
         <v>13</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1010,10 +1010,10 @@
         <v>30</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1049,10 +1049,10 @@
         <v>30</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="190.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1093,10 +1093,10 @@
         <v>30</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="194.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1143,10 +1143,10 @@
         <v>64</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="126.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1190,10 +1190,10 @@
         <v>76</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1207,10 +1207,10 @@
         <v>80</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>81</v>
@@ -1219,16 +1219,16 @@
         <v>82</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -1239,28 +1239,28 @@
         <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>84</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>86</v>
@@ -1269,100 +1269,100 @@
         <v>86</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="151.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>134</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>86</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="O10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="I11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1376,21 +1376,21 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1404,21 +1404,21 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1434,37 +1434,37 @@
     </row>
     <row r="15" spans="1:16" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="O15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to meta data file
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="138">
   <si>
     <t>Layer</t>
   </si>
@@ -450,6 +450,12 @@
   </si>
   <si>
     <t>ICES Quotas for Harp and Hooded Seals. Pacific Walrus PBR - joint with USA - assume this is split equally</t>
+  </si>
+  <si>
+    <t>spp_status_arc2016</t>
+  </si>
+  <si>
+    <t>spp_trend_arc2016</t>
   </si>
 </sst>
 </file>
@@ -840,11 +846,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,6 +1471,16 @@
       </c>
       <c r="P15" s="1" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update trash in layers.csv
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
   <si>
     <t>Layer</t>
   </si>
@@ -468,6 +468,21 @@
   </si>
   <si>
     <t>Scores cross-checked with Global data</t>
+  </si>
+  <si>
+    <t>cw_trash_trend</t>
+  </si>
+  <si>
+    <t>cw_pathogen_trend</t>
+  </si>
+  <si>
+    <t>Proxy of sanitation</t>
+  </si>
+  <si>
+    <t>All data taken from global - using country level data for each</t>
+  </si>
+  <si>
+    <t>Amount of plastic pollution</t>
   </si>
 </sst>
 </file>
@@ -858,11 +873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,21 +1530,71 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>137</v>
       </c>
     </row>
+    <row r="19" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="C14:N14"/>
     <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C19:P19"/>
+    <mergeCell ref="C20:P20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>

<commit_message>
update area_protected_total with new beaufort sea data. remove incorrect bottle nose dolphin from ICO species
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MB4514\Documents\github\arc\circle2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MB4514.IC\Documents\github\arc\circle2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="151">
   <si>
     <t>Layer</t>
   </si>
@@ -483,6 +483,18 @@
   </si>
   <si>
     <t>Amount of plastic pollution</t>
+  </si>
+  <si>
+    <t>iconic_species</t>
+  </si>
+  <si>
+    <t>How iconic species were chosen for each region</t>
+  </si>
+  <si>
+    <t>Species found in North Alaska protected under Marine Mammal Protection Act or Endangered Species Act</t>
+  </si>
+  <si>
+    <t>Arctic Marine Mammals, Ivory Gull</t>
   </si>
 </sst>
 </file>
@@ -873,11 +885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1587,6 +1599,20 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
update ico_list with arctic species trend species
</commit_message>
<xml_diff>
--- a/circle2016/Meta_Data_arc2016.xlsx
+++ b/circle2016/Meta_Data_arc2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="156">
   <si>
     <t>Layer</t>
   </si>
@@ -495,6 +495,21 @@
   </si>
   <si>
     <t>Arctic Marine Mammals, Ivory Gull</t>
+  </si>
+  <si>
+    <t>Globally Iconic and regionally iconic (from Arctic Biodiversity Trends Indicator Species)</t>
+  </si>
+  <si>
+    <t>http://www.npolar.no/en/species/</t>
+  </si>
+  <si>
+    <t>Key svalbard species as listed here</t>
+  </si>
+  <si>
+    <t>http://www.greenland.com/en/about-greenland/nature-climate/fauna-of-greenland/</t>
+  </si>
+  <si>
+    <t>Species considered important on tourism wbesite</t>
   </si>
 </sst>
 </file>
@@ -885,11 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1612,6 +1627,26 @@
       </c>
       <c r="G21" s="1" t="s">
         <v>149</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1654,8 +1689,10 @@
     <hyperlink ref="H12" r:id="rId29"/>
     <hyperlink ref="F12" r:id="rId30"/>
     <hyperlink ref="J12" r:id="rId31"/>
+    <hyperlink ref="L21" r:id="rId32"/>
+    <hyperlink ref="N21" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>